<commit_message>
api for selection; update sort point & sort student
</commit_message>
<xml_diff>
--- a/error-import-demo-student-list.xlsx
+++ b/error-import-demo-student-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boku no\InternshipProject\student-fita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363EA886-00A2-442A-B3EE-605C70009815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F360CD3-0652-4876-B094-8797ABF4BFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0A5968B0-B636-4779-A398-BA415D297B06}"/>
   </bookViews>
@@ -677,7 +677,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>